<commit_message>
truncate sector 96 having a labor reduction of 100% to 99%
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/calibration_data/ERMG_temporary_unemployment.xlsx
+++ b/data/EPNM/interim/calibration_data/ERMG_temporary_unemployment.xlsx
@@ -224,7 +224,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -249,6 +249,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -317,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,6 +337,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,15 +349,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -429,13 +440,13 @@
   </sheetPr>
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BK8" activeCellId="0" sqref="BK8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.53"/>
@@ -888,8 +899,8 @@
       <c r="BH3" s="2" t="n">
         <v>72.0974450386215</v>
       </c>
-      <c r="BK3" s="2" t="n">
-        <v>99.84375</v>
+      <c r="BK3" s="3" t="n">
+        <v>99</v>
       </c>
       <c r="BM3" s="0" t="n">
         <v>31</v>
@@ -1126,8 +1137,8 @@
       <c r="BH5" s="2" t="n">
         <v>86.094867807154</v>
       </c>
-      <c r="BK5" s="2" t="n">
-        <v>100</v>
+      <c r="BK5" s="3" t="n">
+        <v>99</v>
       </c>
       <c r="BM5" s="0" t="n">
         <v>29</v>
@@ -1245,8 +1256,8 @@
       <c r="BH6" s="2" t="n">
         <v>85.1504787961696</v>
       </c>
-      <c r="BK6" s="2" t="n">
-        <v>100</v>
+      <c r="BK6" s="3" t="n">
+        <v>99</v>
       </c>
       <c r="BM6" s="0" t="n">
         <v>24</v>
@@ -1364,8 +1375,8 @@
       <c r="BH7" s="2" t="n">
         <v>84.0239520958084</v>
       </c>
-      <c r="BK7" s="2" t="n">
-        <v>100</v>
+      <c r="BK7" s="3" t="n">
+        <v>99</v>
       </c>
       <c r="BM7" s="0" t="n">
         <v>22</v>
@@ -1732,115 +1743,115 @@
       <c r="A11" s="1" t="n">
         <v>44061</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>2.13016475459329</v>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="4" t="n">
         <v>6.89846047396644</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="4" t="n">
         <v>7.71592225511649</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="4" t="n">
         <v>2.36923831317424</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <v>2.36923831317424</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="N11" s="4" t="n">
         <v>3.19303875586275</v>
       </c>
-      <c r="O11" s="3" t="n">
+      <c r="O11" s="4" t="n">
         <v>3.19303875586275</v>
       </c>
-      <c r="P11" s="3" t="n">
+      <c r="P11" s="4" t="n">
         <v>13.650054433289</v>
       </c>
-      <c r="Q11" s="3" t="n">
+      <c r="Q11" s="4" t="n">
         <v>13.650054433289</v>
       </c>
-      <c r="R11" s="3" t="n">
+      <c r="R11" s="4" t="n">
         <v>5.11772400261609</v>
       </c>
-      <c r="T11" s="3" t="n">
+      <c r="T11" s="4" t="n">
         <v>5.7856001762794</v>
       </c>
-      <c r="V11" s="3" t="n">
+      <c r="V11" s="4" t="n">
         <v>0.206896551724138</v>
       </c>
-      <c r="W11" s="3" t="n">
+      <c r="W11" s="4" t="n">
         <v>1.25789309159112</v>
       </c>
-      <c r="AB11" s="3" t="n">
+      <c r="AB11" s="4" t="n">
         <v>3.12566817256958</v>
       </c>
-      <c r="AD11" s="3" t="n">
+      <c r="AD11" s="4" t="n">
         <v>3.26595358955765</v>
       </c>
       <c r="AE11" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="AF11" s="3" t="n">
+      <c r="AF11" s="4" t="n">
         <v>2.88738019169329</v>
       </c>
-      <c r="AH11" s="3" t="n">
+      <c r="AH11" s="4" t="n">
         <v>4.57259585166562</v>
       </c>
-      <c r="AI11" s="3" t="n">
+      <c r="AI11" s="4" t="n">
         <v>3.21170892599464</v>
       </c>
-      <c r="AK11" s="3" t="n">
+      <c r="AK11" s="4" t="n">
         <v>24.4617773530817</v>
       </c>
-      <c r="AL11" s="3" t="n">
+      <c r="AL11" s="4" t="n">
         <v>4.56897494803632</v>
       </c>
-      <c r="AM11" s="3" t="n">
+      <c r="AM11" s="4" t="n">
         <v>4.56897494803632</v>
       </c>
-      <c r="AN11" s="3" t="n">
+      <c r="AN11" s="4" t="n">
         <v>4.56897494803632</v>
       </c>
-      <c r="AO11" s="3" t="n">
+      <c r="AO11" s="4" t="n">
         <v>4.56897494803632</v>
       </c>
-      <c r="AP11" s="3" t="n">
+      <c r="AP11" s="4" t="n">
         <v>0.402298850574713</v>
       </c>
-      <c r="AQ11" s="3" t="n">
+      <c r="AQ11" s="4" t="n">
         <v>0.402298850574713</v>
       </c>
-      <c r="AR11" s="3" t="n">
+      <c r="AR11" s="4" t="n">
         <v>0.402298850574713</v>
       </c>
-      <c r="AS11" s="3" t="n">
+      <c r="AS11" s="4" t="n">
         <v>0</v>
       </c>
       <c r="AT11" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="AZ11" s="3" t="n">
+      <c r="AZ11" s="4" t="n">
         <v>12.8867046042421</v>
       </c>
-      <c r="BA11" s="3" t="n">
+      <c r="BA11" s="4" t="n">
         <v>69.2809642560266</v>
       </c>
       <c r="BB11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="BG11" s="3" t="n">
+      <c r="BG11" s="4" t="n">
         <v>60.1125509070715</v>
       </c>
-      <c r="BH11" s="3" t="n">
+      <c r="BH11" s="4" t="n">
         <v>60.1125509070715</v>
       </c>
-      <c r="BK11" s="3" t="n">
+      <c r="BK11" s="4" t="n">
         <v>10.8428571428571</v>
       </c>
       <c r="BM11" s="0" t="n">
@@ -1851,115 +1862,115 @@
       <c r="A12" s="1" t="n">
         <v>44096</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>1.49253731343284</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>1.49253731343284</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <v>1.94863204913456</v>
       </c>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="4" t="n">
         <v>6.05306859205776</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="4" t="n">
         <v>8.5968914514916</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="4" t="n">
         <v>1.4736697468311</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="4" t="n">
         <v>1.4736697468311</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="N12" s="4" t="n">
         <v>7.60351583183311</v>
       </c>
-      <c r="O12" s="3" t="n">
+      <c r="O12" s="4" t="n">
         <v>7.60351583183311</v>
       </c>
-      <c r="P12" s="3" t="n">
+      <c r="P12" s="4" t="n">
         <v>10.4502740798747</v>
       </c>
-      <c r="Q12" s="3" t="n">
+      <c r="Q12" s="4" t="n">
         <v>10.4502740798747</v>
       </c>
-      <c r="R12" s="3" t="n">
+      <c r="R12" s="4" t="n">
         <v>3.61459265890779</v>
       </c>
-      <c r="T12" s="3" t="n">
+      <c r="T12" s="4" t="n">
         <v>2.61707078128827</v>
       </c>
-      <c r="V12" s="3" t="n">
+      <c r="V12" s="4" t="n">
         <v>1.40167364016736</v>
       </c>
-      <c r="W12" s="3" t="n">
+      <c r="W12" s="4" t="n">
         <v>2.03678779721848</v>
       </c>
-      <c r="AB12" s="3" t="n">
+      <c r="AB12" s="4" t="n">
         <v>2.46416596814753</v>
       </c>
-      <c r="AD12" s="3" t="n">
+      <c r="AD12" s="4" t="n">
         <v>4.25445705024311</v>
       </c>
       <c r="AE12" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="AF12" s="3" t="n">
+      <c r="AF12" s="4" t="n">
         <v>8.63859516616314</v>
       </c>
-      <c r="AH12" s="3" t="n">
+      <c r="AH12" s="4" t="n">
         <v>1.46396396396396</v>
       </c>
-      <c r="AI12" s="3" t="n">
+      <c r="AI12" s="4" t="n">
         <v>5.57336523125997</v>
       </c>
-      <c r="AK12" s="3" t="n">
+      <c r="AK12" s="4" t="n">
         <v>34.2603795966785</v>
       </c>
-      <c r="AL12" s="3" t="n">
+      <c r="AL12" s="4" t="n">
         <v>2.71989651928504</v>
       </c>
-      <c r="AM12" s="3" t="n">
+      <c r="AM12" s="4" t="n">
         <v>2.71989651928504</v>
       </c>
-      <c r="AN12" s="3" t="n">
+      <c r="AN12" s="4" t="n">
         <v>2.71989651928504</v>
       </c>
-      <c r="AO12" s="3" t="n">
+      <c r="AO12" s="4" t="n">
         <v>2.71989651928504</v>
       </c>
-      <c r="AP12" s="3" t="n">
+      <c r="AP12" s="4" t="n">
         <v>0.0482456140350877</v>
       </c>
-      <c r="AQ12" s="3" t="n">
+      <c r="AQ12" s="4" t="n">
         <v>0.0482456140350877</v>
       </c>
-      <c r="AR12" s="3" t="n">
+      <c r="AR12" s="4" t="n">
         <v>0.0482456140350877</v>
       </c>
-      <c r="AS12" s="3" t="n">
+      <c r="AS12" s="4" t="n">
         <v>15.5844155844156</v>
       </c>
       <c r="AT12" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="AZ12" s="3" t="n">
+      <c r="AZ12" s="4" t="n">
         <v>0.855285376561972</v>
       </c>
-      <c r="BA12" s="3" t="n">
+      <c r="BA12" s="4" t="n">
         <v>63.2489959839357</v>
       </c>
       <c r="BB12" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="BG12" s="3" t="n">
+      <c r="BG12" s="4" t="n">
         <v>58.4554991539763</v>
       </c>
-      <c r="BH12" s="3" t="n">
+      <c r="BH12" s="4" t="n">
         <v>58.4554991539763</v>
       </c>
-      <c r="BK12" s="3" t="n">
+      <c r="BK12" s="4" t="n">
         <v>11.0077519379845</v>
       </c>
       <c r="BM12" s="0" t="n">
@@ -1970,115 +1981,115 @@
       <c r="A13" s="1" t="n">
         <v>44124</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>1.60599571734475</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>1.60599571734475</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="4" t="n">
         <v>2.5197358713295</v>
       </c>
-      <c r="G13" s="3" t="n">
+      <c r="G13" s="4" t="n">
         <v>10.9812082405345</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="4" t="n">
         <v>5.37081189609738</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="4" t="n">
         <v>1.63052661222191</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="4" t="n">
         <v>1.63052661222191</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="N13" s="4" t="n">
         <v>0.49580472921434</v>
       </c>
-      <c r="O13" s="3" t="n">
+      <c r="O13" s="4" t="n">
         <v>0.49580472921434</v>
       </c>
-      <c r="P13" s="3" t="n">
+      <c r="P13" s="4" t="n">
         <v>9.38970171260066</v>
       </c>
-      <c r="Q13" s="3" t="n">
+      <c r="Q13" s="4" t="n">
         <v>9.38970171260066</v>
       </c>
-      <c r="R13" s="3" t="n">
+      <c r="R13" s="4" t="n">
         <v>0.862405805191181</v>
       </c>
-      <c r="T13" s="3" t="n">
+      <c r="T13" s="4" t="n">
         <v>6.54495696498705</v>
       </c>
-      <c r="V13" s="3" t="n">
+      <c r="V13" s="4" t="n">
         <v>3.16375601113642</v>
       </c>
-      <c r="W13" s="3" t="n">
+      <c r="W13" s="4" t="n">
         <v>5.8028028028028</v>
       </c>
-      <c r="AB13" s="3" t="n">
+      <c r="AB13" s="4" t="n">
         <v>2.3671096345515</v>
       </c>
-      <c r="AD13" s="3" t="n">
+      <c r="AD13" s="4" t="n">
         <v>6.0143286750398</v>
       </c>
       <c r="AE13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AF13" s="3" t="n">
+      <c r="AF13" s="4" t="n">
         <v>10.8547655068079</v>
       </c>
-      <c r="AH13" s="3" t="n">
+      <c r="AH13" s="4" t="n">
         <v>5.62756876383181</v>
       </c>
-      <c r="AI13" s="3" t="n">
+      <c r="AI13" s="4" t="n">
         <v>3.54660207120316</v>
       </c>
-      <c r="AK13" s="3" t="n">
+      <c r="AK13" s="4" t="n">
         <v>59.5436218282934</v>
       </c>
-      <c r="AL13" s="3" t="n">
+      <c r="AL13" s="4" t="n">
         <v>3.08000782472613</v>
       </c>
-      <c r="AM13" s="3" t="n">
+      <c r="AM13" s="4" t="n">
         <v>3.08000782472613</v>
       </c>
-      <c r="AN13" s="3" t="n">
+      <c r="AN13" s="4" t="n">
         <v>3.08000782472613</v>
       </c>
-      <c r="AO13" s="3" t="n">
+      <c r="AO13" s="4" t="n">
         <v>3.08000782472613</v>
       </c>
-      <c r="AP13" s="3" t="n">
+      <c r="AP13" s="4" t="n">
         <v>0.0433036768758366</v>
       </c>
-      <c r="AQ13" s="3" t="n">
+      <c r="AQ13" s="4" t="n">
         <v>0.0433036768758366</v>
       </c>
-      <c r="AR13" s="3" t="n">
+      <c r="AR13" s="4" t="n">
         <v>0.0433036768758366</v>
       </c>
-      <c r="AS13" s="3" t="n">
+      <c r="AS13" s="4" t="n">
         <v>2.73556231003039</v>
       </c>
       <c r="AT13" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="AZ13" s="3" t="n">
+      <c r="AZ13" s="4" t="n">
         <v>4.66833890746934</v>
       </c>
-      <c r="BA13" s="3" t="n">
+      <c r="BA13" s="4" t="n">
         <v>68.5383064516129</v>
       </c>
       <c r="BB13" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="BG13" s="3" t="n">
+      <c r="BG13" s="4" t="n">
         <v>61.3140333660452</v>
       </c>
-      <c r="BH13" s="3" t="n">
+      <c r="BH13" s="4" t="n">
         <v>61.3140333660452</v>
       </c>
-      <c r="BK13" s="3" t="n">
+      <c r="BK13" s="4" t="n">
         <v>14.7250859106529</v>
       </c>
       <c r="BM13" s="0" t="n">
@@ -2089,115 +2100,115 @@
       <c r="A14" s="1" t="n">
         <v>44145</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>5.33536585365854</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="4" t="n">
         <v>5.33536585365854</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>3.39375629405841</v>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="4" t="n">
         <v>7.76861451460886</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="4" t="n">
         <v>4.5785726113595</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="4" t="n">
         <v>0.953167839940719</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="4" t="n">
         <v>0.953167839940719</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="N14" s="4" t="n">
         <v>1.82595680992089</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="O14" s="4" t="n">
         <v>1.82595680992089</v>
       </c>
-      <c r="P14" s="3" t="n">
+      <c r="P14" s="4" t="n">
         <v>6.34461487162388</v>
       </c>
-      <c r="Q14" s="3" t="n">
+      <c r="Q14" s="4" t="n">
         <v>6.34461487162388</v>
       </c>
-      <c r="R14" s="3" t="n">
+      <c r="R14" s="4" t="n">
         <v>2.57590841214535</v>
       </c>
-      <c r="T14" s="3" t="n">
+      <c r="T14" s="4" t="n">
         <v>8.26009713701431</v>
       </c>
-      <c r="V14" s="3" t="n">
+      <c r="V14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="W14" s="3" t="n">
+      <c r="W14" s="4" t="n">
         <v>5.71321038765525</v>
       </c>
-      <c r="AB14" s="3" t="n">
+      <c r="AB14" s="4" t="n">
         <v>4.35640606767795</v>
       </c>
-      <c r="AD14" s="3" t="n">
+      <c r="AD14" s="4" t="n">
         <v>8.82039781591264</v>
       </c>
       <c r="AE14" s="0" t="n">
         <v>23.5</v>
       </c>
-      <c r="AF14" s="3" t="n">
+      <c r="AF14" s="4" t="n">
         <v>6.03728813559322</v>
       </c>
-      <c r="AH14" s="3" t="n">
+      <c r="AH14" s="4" t="n">
         <v>1.14823348694316</v>
       </c>
-      <c r="AI14" s="3" t="n">
+      <c r="AI14" s="4" t="n">
         <v>2.1379726468222</v>
       </c>
-      <c r="AK14" s="3" t="n">
+      <c r="AK14" s="4" t="n">
         <v>70.0507767215395</v>
       </c>
-      <c r="AL14" s="3" t="n">
+      <c r="AL14" s="4" t="n">
         <v>3.21329822251481</v>
       </c>
-      <c r="AM14" s="3" t="n">
+      <c r="AM14" s="4" t="n">
         <v>3.21329822251481</v>
       </c>
-      <c r="AN14" s="3" t="n">
+      <c r="AN14" s="4" t="n">
         <v>3.21329822251481</v>
       </c>
-      <c r="AO14" s="3" t="n">
+      <c r="AO14" s="4" t="n">
         <v>3.21329822251481</v>
       </c>
-      <c r="AP14" s="3" t="n">
+      <c r="AP14" s="4" t="n">
         <v>0.812695109261186</v>
       </c>
-      <c r="AQ14" s="3" t="n">
+      <c r="AQ14" s="4" t="n">
         <v>0.812695109261186</v>
       </c>
-      <c r="AR14" s="3" t="n">
+      <c r="AR14" s="4" t="n">
         <v>0.812695109261186</v>
       </c>
-      <c r="AS14" s="3" t="n">
+      <c r="AS14" s="4" t="n">
         <v>7.16452991452992</v>
       </c>
       <c r="AT14" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="AZ14" s="3" t="n">
+      <c r="AZ14" s="4" t="n">
         <v>4.8155737704918</v>
       </c>
-      <c r="BA14" s="3" t="n">
+      <c r="BA14" s="4" t="n">
         <v>45.3097893432466</v>
       </c>
       <c r="BB14" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="BG14" s="3" t="n">
+      <c r="BG14" s="4" t="n">
         <v>57.003164556962</v>
       </c>
-      <c r="BH14" s="3" t="n">
+      <c r="BH14" s="4" t="n">
         <v>57.003164556962</v>
       </c>
-      <c r="BK14" s="3" t="n">
+      <c r="BK14" s="4" t="n">
         <v>85.2494802494803</v>
       </c>
       <c r="BM14" s="0" t="n">
@@ -2208,115 +2219,115 @@
       <c r="A15" s="1" t="n">
         <v>44173</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>0.660660660660661</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="4" t="n">
         <v>0.660660660660661</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="4" t="n">
         <v>2.20662170447578</v>
       </c>
-      <c r="G15" s="3" t="n">
+      <c r="G15" s="4" t="n">
         <v>9.02056074766355</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="4" t="n">
         <v>5.65770736917052</v>
       </c>
-      <c r="L15" s="3" t="n">
+      <c r="L15" s="4" t="n">
         <v>0.890104841067625</v>
       </c>
-      <c r="M15" s="3" t="n">
+      <c r="M15" s="4" t="n">
         <v>0.890104841067625</v>
       </c>
-      <c r="N15" s="3" t="n">
+      <c r="N15" s="4" t="n">
         <v>5.34887924801157</v>
       </c>
-      <c r="O15" s="3" t="n">
+      <c r="O15" s="4" t="n">
         <v>5.34887924801157</v>
       </c>
-      <c r="P15" s="3" t="n">
+      <c r="P15" s="4" t="n">
         <v>3.67263901777429</v>
       </c>
-      <c r="Q15" s="3" t="n">
+      <c r="Q15" s="4" t="n">
         <v>3.67263901777429</v>
       </c>
-      <c r="R15" s="3" t="n">
+      <c r="R15" s="4" t="n">
         <v>1.04982206405694</v>
       </c>
-      <c r="T15" s="3" t="n">
+      <c r="T15" s="4" t="n">
         <v>5.83274647887324</v>
       </c>
-      <c r="V15" s="3" t="n">
+      <c r="V15" s="4" t="n">
         <v>4.31769340974212</v>
       </c>
-      <c r="W15" s="3" t="n">
+      <c r="W15" s="4" t="n">
         <v>9.5592485549133</v>
       </c>
-      <c r="AB15" s="3" t="n">
+      <c r="AB15" s="4" t="n">
         <v>2.18907579198583</v>
       </c>
-      <c r="AD15" s="3" t="n">
+      <c r="AD15" s="4" t="n">
         <v>9.94964219454015</v>
       </c>
       <c r="AE15" s="0" t="n">
         <v>12.5</v>
       </c>
-      <c r="AF15" s="3" t="n">
+      <c r="AF15" s="4" t="n">
         <v>6.11378205128205</v>
       </c>
-      <c r="AH15" s="3" t="n">
+      <c r="AH15" s="4" t="n">
         <v>54.6974608319827</v>
       </c>
-      <c r="AI15" s="3" t="n">
+      <c r="AI15" s="4" t="n">
         <v>2.40375885236971</v>
       </c>
-      <c r="AK15" s="3" t="n">
+      <c r="AK15" s="4" t="n">
         <v>72.8987194412107</v>
       </c>
-      <c r="AL15" s="3" t="n">
+      <c r="AL15" s="4" t="n">
         <v>1.99974460477589</v>
       </c>
-      <c r="AM15" s="3" t="n">
+      <c r="AM15" s="4" t="n">
         <v>1.99974460477589</v>
       </c>
-      <c r="AN15" s="3" t="n">
+      <c r="AN15" s="4" t="n">
         <v>1.99974460477589</v>
       </c>
-      <c r="AO15" s="3" t="n">
+      <c r="AO15" s="4" t="n">
         <v>1.99974460477589</v>
       </c>
-      <c r="AP15" s="3" t="n">
+      <c r="AP15" s="4" t="n">
         <v>2.95952380952381</v>
       </c>
-      <c r="AQ15" s="3" t="n">
+      <c r="AQ15" s="4" t="n">
         <v>2.95952380952381</v>
       </c>
-      <c r="AR15" s="3" t="n">
+      <c r="AR15" s="4" t="n">
         <v>2.95952380952381</v>
       </c>
-      <c r="AS15" s="3" t="n">
+      <c r="AS15" s="4" t="n">
         <v>5.74538258575198</v>
       </c>
       <c r="AT15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AZ15" s="3" t="n">
+      <c r="AZ15" s="4" t="n">
         <v>1.99570815450644</v>
       </c>
-      <c r="BA15" s="3" t="n">
+      <c r="BA15" s="4" t="n">
         <v>64.6815286624204</v>
       </c>
       <c r="BB15" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="BG15" s="3" t="n">
+      <c r="BG15" s="4" t="n">
         <v>62.4537444933921</v>
       </c>
-      <c r="BH15" s="3" t="n">
+      <c r="BH15" s="4" t="n">
         <v>62.4537444933921</v>
       </c>
-      <c r="BK15" s="3" t="n">
+      <c r="BK15" s="4" t="n">
         <v>83.4959742351047</v>
       </c>
       <c r="BM15" s="0" t="n">
@@ -2327,115 +2338,115 @@
       <c r="A16" s="1" t="n">
         <v>44208</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>0.204460966542751</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="4" t="n">
         <v>0.204460966542751</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>5.40905409054091</v>
       </c>
-      <c r="G16" s="3" t="n">
+      <c r="G16" s="4" t="n">
         <v>5.66405917864127</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <v>2.41957104557641</v>
       </c>
-      <c r="L16" s="3" t="n">
+      <c r="L16" s="4" t="n">
         <v>0.451586136465182</v>
       </c>
-      <c r="M16" s="3" t="n">
+      <c r="M16" s="4" t="n">
         <v>0.451586136465182</v>
       </c>
-      <c r="N16" s="3" t="n">
+      <c r="N16" s="4" t="n">
         <v>2.58896338318721</v>
       </c>
-      <c r="O16" s="3" t="n">
+      <c r="O16" s="4" t="n">
         <v>2.58896338318721</v>
       </c>
-      <c r="P16" s="3" t="n">
+      <c r="P16" s="4" t="n">
         <v>3.10443218565722</v>
       </c>
-      <c r="Q16" s="3" t="n">
+      <c r="Q16" s="4" t="n">
         <v>3.10443218565722</v>
       </c>
-      <c r="R16" s="3" t="n">
+      <c r="R16" s="4" t="n">
         <v>4.55696202531646</v>
       </c>
-      <c r="T16" s="3" t="n">
+      <c r="T16" s="4" t="n">
         <v>2.17545719586536</v>
       </c>
-      <c r="V16" s="3" t="n">
+      <c r="V16" s="4" t="n">
         <v>1.26284289276808</v>
       </c>
-      <c r="W16" s="3" t="n">
+      <c r="W16" s="4" t="n">
         <v>4.79103834554072</v>
       </c>
-      <c r="AB16" s="3" t="n">
+      <c r="AB16" s="4" t="n">
         <v>1.90340358978178</v>
       </c>
-      <c r="AD16" s="3" t="n">
+      <c r="AD16" s="4" t="n">
         <v>4.9629217059198</v>
       </c>
       <c r="AE16" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AF16" s="3" t="n">
+      <c r="AF16" s="4" t="n">
         <v>21.5538628944505</v>
       </c>
-      <c r="AH16" s="3" t="n">
+      <c r="AH16" s="4" t="n">
         <v>22.3255352894528</v>
       </c>
-      <c r="AI16" s="3" t="n">
+      <c r="AI16" s="4" t="n">
         <v>2.68310265282584</v>
       </c>
-      <c r="AK16" s="3" t="n">
+      <c r="AK16" s="4" t="n">
         <v>71.3916191311979</v>
       </c>
-      <c r="AL16" s="3" t="n">
+      <c r="AL16" s="4" t="n">
         <v>1.91215799218268</v>
       </c>
-      <c r="AM16" s="3" t="n">
+      <c r="AM16" s="4" t="n">
         <v>1.91215799218268</v>
       </c>
-      <c r="AN16" s="3" t="n">
+      <c r="AN16" s="4" t="n">
         <v>1.91215799218268</v>
       </c>
-      <c r="AO16" s="3" t="n">
+      <c r="AO16" s="4" t="n">
         <v>1.91215799218268</v>
       </c>
-      <c r="AP16" s="3" t="n">
+      <c r="AP16" s="4" t="n">
         <v>0.22241847826087</v>
       </c>
-      <c r="AQ16" s="3" t="n">
+      <c r="AQ16" s="4" t="n">
         <v>0.22241847826087</v>
       </c>
-      <c r="AR16" s="3" t="n">
+      <c r="AR16" s="4" t="n">
         <v>0.22241847826087</v>
       </c>
-      <c r="AS16" s="3" t="n">
+      <c r="AS16" s="4" t="n">
         <v>1.61206896551724</v>
       </c>
       <c r="AT16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AZ16" s="3" t="n">
+      <c r="AZ16" s="4" t="n">
         <v>1.57286212914485</v>
       </c>
-      <c r="BA16" s="3" t="n">
+      <c r="BA16" s="4" t="n">
         <v>40.8438818565401</v>
       </c>
       <c r="BB16" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="BG16" s="3" t="n">
+      <c r="BG16" s="4" t="n">
         <v>46.8894389438944</v>
       </c>
-      <c r="BH16" s="3" t="n">
+      <c r="BH16" s="4" t="n">
         <v>46.8894389438944</v>
       </c>
-      <c r="BK16" s="3" t="n">
+      <c r="BK16" s="4" t="n">
         <v>92.0143149284253</v>
       </c>
       <c r="BM16" s="0" t="n">
@@ -2446,115 +2457,115 @@
       <c r="A17" s="1" t="n">
         <v>44236</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>1.72594142259414</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="4" t="n">
         <v>1.72594142259414</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="4" t="n">
         <v>7.01038794485412</v>
       </c>
-      <c r="G17" s="3" t="n">
+      <c r="G17" s="4" t="n">
         <v>2.24369621017666</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="4" t="n">
         <v>9.39545676599902</v>
       </c>
-      <c r="L17" s="3" t="n">
+      <c r="L17" s="4" t="n">
         <v>1.54096477794793</v>
       </c>
-      <c r="M17" s="3" t="n">
+      <c r="M17" s="4" t="n">
         <v>1.54096477794793</v>
       </c>
-      <c r="N17" s="3" t="n">
+      <c r="N17" s="4" t="n">
         <v>2.53907703758839</v>
       </c>
-      <c r="O17" s="3" t="n">
+      <c r="O17" s="4" t="n">
         <v>2.53907703758839</v>
       </c>
-      <c r="P17" s="3" t="n">
+      <c r="P17" s="4" t="n">
         <v>6.31197859279081</v>
       </c>
-      <c r="Q17" s="3" t="n">
+      <c r="Q17" s="4" t="n">
         <v>6.31197859279081</v>
       </c>
-      <c r="R17" s="3" t="n">
+      <c r="R17" s="4" t="n">
         <v>1.19209265175719</v>
       </c>
-      <c r="T17" s="3" t="n">
+      <c r="T17" s="4" t="n">
         <v>2.01022436807725</v>
       </c>
-      <c r="V17" s="3" t="n">
+      <c r="V17" s="4" t="n">
         <v>0.547958978483813</v>
       </c>
-      <c r="W17" s="3" t="n">
+      <c r="W17" s="4" t="n">
         <v>4.91837588949351</v>
       </c>
-      <c r="AB17" s="3" t="n">
+      <c r="AB17" s="4" t="n">
         <v>2.02833251790241</v>
       </c>
-      <c r="AD17" s="3" t="n">
+      <c r="AD17" s="4" t="n">
         <v>6.95749856897539</v>
       </c>
       <c r="AE17" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="AF17" s="3" t="n">
+      <c r="AF17" s="4" t="n">
         <v>5.90909090909091</v>
       </c>
-      <c r="AH17" s="3" t="n">
+      <c r="AH17" s="4" t="n">
         <v>19.7287299630086</v>
       </c>
-      <c r="AI17" s="3" t="n">
+      <c r="AI17" s="4" t="n">
         <v>2.79183119447187</v>
       </c>
-      <c r="AK17" s="3" t="n">
+      <c r="AK17" s="4" t="n">
         <v>60.5058688806184</v>
       </c>
-      <c r="AL17" s="3" t="n">
+      <c r="AL17" s="4" t="n">
         <v>2.47687754347022</v>
       </c>
-      <c r="AM17" s="3" t="n">
+      <c r="AM17" s="4" t="n">
         <v>2.47687754347022</v>
       </c>
-      <c r="AN17" s="3" t="n">
+      <c r="AN17" s="4" t="n">
         <v>2.47687754347022</v>
       </c>
-      <c r="AO17" s="3" t="n">
+      <c r="AO17" s="4" t="n">
         <v>2.47687754347022</v>
       </c>
-      <c r="AP17" s="3" t="n">
+      <c r="AP17" s="4" t="n">
         <v>0.0965804066543438</v>
       </c>
-      <c r="AQ17" s="3" t="n">
+      <c r="AQ17" s="4" t="n">
         <v>0.0965804066543438</v>
       </c>
-      <c r="AR17" s="3" t="n">
+      <c r="AR17" s="4" t="n">
         <v>0.0965804066543438</v>
       </c>
-      <c r="AS17" s="3" t="n">
+      <c r="AS17" s="4" t="n">
         <v>5.73991031390135</v>
       </c>
       <c r="AT17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AZ17" s="3" t="n">
+      <c r="AZ17" s="4" t="n">
         <v>2.16924910607866</v>
       </c>
-      <c r="BA17" s="3" t="n">
+      <c r="BA17" s="4" t="n">
         <v>70.2730109204368</v>
       </c>
       <c r="BB17" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="BG17" s="3" t="n">
+      <c r="BG17" s="4" t="n">
         <v>56.4194139194139</v>
       </c>
-      <c r="BH17" s="3" t="n">
+      <c r="BH17" s="4" t="n">
         <v>56.4194139194139</v>
       </c>
-      <c r="BK17" s="3" t="n">
+      <c r="BK17" s="4" t="n">
         <v>89</v>
       </c>
       <c r="BM17" s="0" t="n">
@@ -2565,115 +2576,115 @@
       <c r="A18" s="1" t="n">
         <v>44271</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="4" t="n">
         <v>2.36486486486486</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="4" t="n">
         <v>2.36486486486486</v>
       </c>
-      <c r="F18" s="3" t="n">
+      <c r="F18" s="4" t="n">
         <v>4.60835008222182</v>
       </c>
-      <c r="G18" s="3" t="n">
+      <c r="G18" s="4" t="n">
         <v>3.15904139433551</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="4" t="n">
         <v>14.2099091175608</v>
       </c>
-      <c r="L18" s="3" t="n">
+      <c r="L18" s="4" t="n">
         <v>0.872440273037543</v>
       </c>
-      <c r="M18" s="3" t="n">
+      <c r="M18" s="4" t="n">
         <v>0.872440273037543</v>
       </c>
-      <c r="N18" s="3" t="n">
+      <c r="N18" s="4" t="n">
         <v>2.47296322999279</v>
       </c>
-      <c r="O18" s="3" t="n">
+      <c r="O18" s="4" t="n">
         <v>2.47296322999279</v>
       </c>
-      <c r="P18" s="3" t="n">
+      <c r="P18" s="4" t="n">
         <v>3.31036168132942</v>
       </c>
-      <c r="Q18" s="3" t="n">
+      <c r="Q18" s="4" t="n">
         <v>3.31036168132942</v>
       </c>
-      <c r="R18" s="3" t="n">
+      <c r="R18" s="4" t="n">
         <v>1.57685762904141</v>
       </c>
-      <c r="T18" s="3" t="n">
+      <c r="T18" s="4" t="n">
         <v>1.74349872675361</v>
       </c>
-      <c r="V18" s="3" t="n">
+      <c r="V18" s="4" t="n">
         <v>2.72331154684096</v>
       </c>
-      <c r="W18" s="3" t="n">
+      <c r="W18" s="4" t="n">
         <v>6.94990488268865</v>
       </c>
-      <c r="AB18" s="3" t="n">
+      <c r="AB18" s="4" t="n">
         <v>1.22086118839015</v>
       </c>
-      <c r="AD18" s="3" t="n">
+      <c r="AD18" s="4" t="n">
         <v>5.91094295692666</v>
       </c>
       <c r="AE18" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AF18" s="3" t="n">
+      <c r="AF18" s="4" t="n">
         <v>40.7352941176471</v>
       </c>
-      <c r="AH18" s="3" t="n">
+      <c r="AH18" s="4" t="n">
         <v>15.8610271903323</v>
       </c>
-      <c r="AI18" s="3" t="n">
+      <c r="AI18" s="4" t="n">
         <v>2.39155693261038</v>
       </c>
-      <c r="AK18" s="3" t="n">
+      <c r="AK18" s="4" t="n">
         <v>76.5192307692308</v>
       </c>
-      <c r="AL18" s="3" t="n">
+      <c r="AL18" s="4" t="n">
         <v>1.32193821546182</v>
       </c>
-      <c r="AM18" s="3" t="n">
+      <c r="AM18" s="4" t="n">
         <v>1.32193821546182</v>
       </c>
-      <c r="AN18" s="3" t="n">
+      <c r="AN18" s="4" t="n">
         <v>1.32193821546182</v>
       </c>
-      <c r="AO18" s="3" t="n">
+      <c r="AO18" s="4" t="n">
         <v>1.32193821546182</v>
       </c>
-      <c r="AP18" s="3" t="n">
+      <c r="AP18" s="4" t="n">
         <v>0.364838757616288</v>
       </c>
-      <c r="AQ18" s="3" t="n">
+      <c r="AQ18" s="4" t="n">
         <v>0.364838757616288</v>
       </c>
-      <c r="AR18" s="3" t="n">
+      <c r="AR18" s="4" t="n">
         <v>0.364838757616288</v>
       </c>
-      <c r="AS18" s="3" t="n">
+      <c r="AS18" s="4" t="n">
         <v>2.66924564796905</v>
       </c>
       <c r="AT18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AZ18" s="3" t="n">
+      <c r="AZ18" s="4" t="n">
         <v>1.09357881923311</v>
       </c>
-      <c r="BA18" s="3" t="n">
+      <c r="BA18" s="4" t="n">
         <v>64.6098829648895</v>
       </c>
       <c r="BB18" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="BG18" s="3" t="n">
+      <c r="BG18" s="4" t="n">
         <v>46.7102552619794</v>
       </c>
-      <c r="BH18" s="3" t="n">
+      <c r="BH18" s="4" t="n">
         <v>46.7102552619794</v>
       </c>
-      <c r="BK18" s="3" t="n">
+      <c r="BK18" s="4" t="n">
         <v>11.304347826087</v>
       </c>
       <c r="BM18" s="0" t="n">
@@ -2684,115 +2695,115 @@
       <c r="A19" s="1" t="n">
         <v>44306</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="4" t="n">
         <v>4.77356181150551</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="4" t="n">
         <v>4.77356181150551</v>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="4" t="n">
         <v>7.06175680859225</v>
       </c>
-      <c r="G19" s="3" t="n">
+      <c r="G19" s="4" t="n">
         <v>4.25785032507954</v>
       </c>
-      <c r="I19" s="3" t="n">
+      <c r="I19" s="4" t="n">
         <v>10.4211733857752</v>
       </c>
-      <c r="L19" s="3" t="n">
+      <c r="L19" s="4" t="n">
         <v>1.47115482104836</v>
       </c>
-      <c r="M19" s="3" t="n">
+      <c r="M19" s="4" t="n">
         <v>1.47115482104836</v>
       </c>
-      <c r="N19" s="3" t="n">
+      <c r="N19" s="4" t="n">
         <v>0.408041401273885</v>
       </c>
-      <c r="O19" s="3" t="n">
+      <c r="O19" s="4" t="n">
         <v>0.408041401273885</v>
       </c>
-      <c r="P19" s="3" t="n">
+      <c r="P19" s="4" t="n">
         <v>3.82786214422115</v>
       </c>
-      <c r="Q19" s="3" t="n">
+      <c r="Q19" s="4" t="n">
         <v>3.82786214422115</v>
       </c>
-      <c r="R19" s="3" t="n">
+      <c r="R19" s="4" t="n">
         <v>1.77496038034865</v>
       </c>
-      <c r="T19" s="3" t="n">
+      <c r="T19" s="4" t="n">
         <v>3.13403684161807</v>
       </c>
-      <c r="V19" s="3" t="n">
+      <c r="V19" s="4" t="n">
         <v>4.52104499274311</v>
       </c>
-      <c r="W19" s="3" t="n">
+      <c r="W19" s="4" t="n">
         <v>6.20337109698812</v>
       </c>
-      <c r="AB19" s="3" t="n">
+      <c r="AB19" s="4" t="n">
         <v>0.929512122119126</v>
       </c>
-      <c r="AD19" s="3" t="n">
+      <c r="AD19" s="4" t="n">
         <v>4.46484549932826</v>
       </c>
       <c r="AE19" s="0" t="n">
         <v>12.5</v>
       </c>
-      <c r="AF19" s="3" t="n">
+      <c r="AF19" s="4" t="n">
         <v>11.5492957746479</v>
       </c>
-      <c r="AH19" s="3" t="n">
+      <c r="AH19" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="AI19" s="3" t="n">
+      <c r="AI19" s="4" t="n">
         <v>1.03503696560591</v>
       </c>
-      <c r="AK19" s="3" t="n">
+      <c r="AK19" s="4" t="n">
         <v>58.8388558482016</v>
       </c>
-      <c r="AL19" s="3" t="n">
+      <c r="AL19" s="4" t="n">
         <v>2.35841625207297</v>
       </c>
-      <c r="AM19" s="3" t="n">
+      <c r="AM19" s="4" t="n">
         <v>2.35841625207297</v>
       </c>
-      <c r="AN19" s="3" t="n">
+      <c r="AN19" s="4" t="n">
         <v>2.35841625207297</v>
       </c>
-      <c r="AO19" s="3" t="n">
+      <c r="AO19" s="4" t="n">
         <v>2.35841625207297</v>
       </c>
-      <c r="AP19" s="3" t="n">
+      <c r="AP19" s="4" t="n">
         <v>0.112982744453574</v>
       </c>
-      <c r="AQ19" s="3" t="n">
+      <c r="AQ19" s="4" t="n">
         <v>0.112982744453574</v>
       </c>
-      <c r="AR19" s="3" t="n">
+      <c r="AR19" s="4" t="n">
         <v>0.112982744453574</v>
       </c>
-      <c r="AS19" s="3" t="n">
+      <c r="AS19" s="4" t="n">
         <v>1.23022847100176</v>
       </c>
       <c r="AT19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AZ19" s="3" t="n">
+      <c r="AZ19" s="4" t="n">
         <v>1.46890061969245</v>
       </c>
-      <c r="BA19" s="3" t="n">
+      <c r="BA19" s="4" t="n">
         <v>57.8392007611798</v>
       </c>
       <c r="BB19" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="BG19" s="3" t="n">
+      <c r="BG19" s="4" t="n">
         <v>47.0383928571429</v>
       </c>
-      <c r="BH19" s="3" t="n">
+      <c r="BH19" s="4" t="n">
         <v>47.0383928571429</v>
       </c>
-      <c r="BK19" s="3" t="n">
+      <c r="BK19" s="4" t="n">
         <v>72.1212121212121</v>
       </c>
       <c r="BM19" s="0" t="n">
@@ -2803,115 +2814,115 @@
       <c r="A20" s="1" t="n">
         <v>44341</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>4.52883263009845</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="4" t="n">
         <v>4.52883263009845</v>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="4" t="n">
         <v>3.44662155337845</v>
       </c>
-      <c r="G20" s="3" t="n">
+      <c r="G20" s="4" t="n">
         <v>2.27621483375959</v>
       </c>
-      <c r="I20" s="3" t="n">
+      <c r="I20" s="4" t="n">
         <v>8.65934449093445</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="L20" s="4" t="n">
         <v>0.411349027287046</v>
       </c>
-      <c r="M20" s="3" t="n">
+      <c r="M20" s="4" t="n">
         <v>0.411349027287046</v>
       </c>
-      <c r="N20" s="3" t="n">
+      <c r="N20" s="4" t="n">
         <v>0.0841143955779861</v>
       </c>
-      <c r="O20" s="3" t="n">
+      <c r="O20" s="4" t="n">
         <v>0.0841143955779861</v>
       </c>
-      <c r="P20" s="3" t="n">
+      <c r="P20" s="4" t="n">
         <v>1.97914225451137</v>
       </c>
-      <c r="Q20" s="3" t="n">
+      <c r="Q20" s="4" t="n">
         <v>1.97914225451137</v>
       </c>
-      <c r="R20" s="3" t="n">
+      <c r="R20" s="4" t="n">
         <v>0.887480190174327</v>
       </c>
-      <c r="T20" s="3" t="n">
+      <c r="T20" s="4" t="n">
         <v>3.98175031107424</v>
       </c>
-      <c r="V20" s="3" t="n">
+      <c r="V20" s="4" t="n">
         <v>0.0642523364485981</v>
       </c>
-      <c r="W20" s="3" t="n">
+      <c r="W20" s="4" t="n">
         <v>5.98925092374874</v>
       </c>
-      <c r="AB20" s="3" t="n">
+      <c r="AB20" s="4" t="n">
         <v>0.536582379232229</v>
       </c>
-      <c r="AD20" s="3" t="n">
+      <c r="AD20" s="4" t="n">
         <v>2.57165149544863</v>
       </c>
       <c r="AE20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AF20" s="3" t="n">
+      <c r="AF20" s="4" t="n">
         <v>59.0601503759399</v>
       </c>
-      <c r="AH20" s="3" t="n">
+      <c r="AH20" s="4" t="n">
         <v>19.6540880503145</v>
       </c>
-      <c r="AI20" s="3" t="n">
+      <c r="AI20" s="4" t="n">
         <v>4.02805611222445</v>
       </c>
-      <c r="AK20" s="3" t="n">
+      <c r="AK20" s="4" t="n">
         <v>42.9572719802794</v>
       </c>
-      <c r="AL20" s="3" t="n">
+      <c r="AL20" s="4" t="n">
         <v>0.581500213271586</v>
       </c>
-      <c r="AM20" s="3" t="n">
+      <c r="AM20" s="4" t="n">
         <v>0.581500213271586</v>
       </c>
-      <c r="AN20" s="3" t="n">
+      <c r="AN20" s="4" t="n">
         <v>0.581500213271586</v>
       </c>
-      <c r="AO20" s="3" t="n">
+      <c r="AO20" s="4" t="n">
         <v>0.581500213271586</v>
       </c>
-      <c r="AP20" s="3" t="n">
+      <c r="AP20" s="4" t="n">
         <v>2.26415094339623</v>
       </c>
-      <c r="AQ20" s="3" t="n">
+      <c r="AQ20" s="4" t="n">
         <v>2.26415094339623</v>
       </c>
-      <c r="AR20" s="3" t="n">
+      <c r="AR20" s="4" t="n">
         <v>2.26415094339623</v>
       </c>
-      <c r="AS20" s="3" t="n">
+      <c r="AS20" s="4" t="n">
         <v>0.294117647058824</v>
       </c>
       <c r="AT20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AZ20" s="3" t="n">
+      <c r="AZ20" s="4" t="n">
         <v>0.25899764547595</v>
       </c>
-      <c r="BA20" s="3" t="n">
+      <c r="BA20" s="4" t="n">
         <v>51.958174904943</v>
       </c>
       <c r="BB20" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="BG20" s="3" t="n">
+      <c r="BG20" s="4" t="n">
         <v>20.3025682182986</v>
       </c>
-      <c r="BH20" s="3" t="n">
+      <c r="BH20" s="4" t="n">
         <v>20.3025682182986</v>
       </c>
-      <c r="BK20" s="3" t="n">
+      <c r="BK20" s="4" t="n">
         <v>3.84615384615385</v>
       </c>
       <c r="BM20" s="0" t="n">
@@ -2922,115 +2933,115 @@
       <c r="A21" s="1" t="n">
         <v>44369</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
         <v>1.46478873239437</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="4" t="n">
         <v>1.46478873239437</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>1.18225831641418</v>
       </c>
-      <c r="G21" s="3" t="n">
+      <c r="G21" s="4" t="n">
         <v>3.4156378600823</v>
       </c>
-      <c r="I21" s="3" t="n">
+      <c r="I21" s="4" t="n">
         <v>10.4122396940077</v>
       </c>
-      <c r="L21" s="3" t="n">
+      <c r="L21" s="4" t="n">
         <v>0.812386307259798</v>
       </c>
-      <c r="M21" s="3" t="n">
+      <c r="M21" s="4" t="n">
         <v>0.812386307259798</v>
       </c>
-      <c r="N21" s="3" t="n">
+      <c r="N21" s="4" t="n">
         <v>0.37397157816006</v>
       </c>
-      <c r="O21" s="3" t="n">
+      <c r="O21" s="4" t="n">
         <v>0.37397157816006</v>
       </c>
-      <c r="P21" s="3" t="n">
+      <c r="P21" s="4" t="n">
         <v>3.32439678284182</v>
       </c>
-      <c r="Q21" s="3" t="n">
+      <c r="Q21" s="4" t="n">
         <v>3.32439678284182</v>
       </c>
-      <c r="R21" s="3" t="n">
+      <c r="R21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="T21" s="3" t="n">
+      <c r="T21" s="4" t="n">
         <v>0.881666985280061</v>
       </c>
-      <c r="V21" s="3" t="n">
+      <c r="V21" s="4" t="n">
         <v>0.0471380471380471</v>
       </c>
-      <c r="W21" s="3" t="n">
+      <c r="W21" s="4" t="n">
         <v>9.9349593495935</v>
       </c>
-      <c r="AB21" s="3" t="n">
+      <c r="AB21" s="4" t="n">
         <v>0.590070757452732</v>
       </c>
-      <c r="AD21" s="3" t="n">
+      <c r="AD21" s="4" t="n">
         <v>1.47817119284978</v>
       </c>
       <c r="AE21" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AF21" s="3" t="n">
+      <c r="AF21" s="4" t="n">
         <v>1.93470374848851</v>
       </c>
-      <c r="AH21" s="3" t="n">
+      <c r="AH21" s="4" t="n">
         <v>9.97715156130998</v>
       </c>
-      <c r="AI21" s="3" t="n">
+      <c r="AI21" s="4" t="n">
         <v>0.330013200528021</v>
       </c>
-      <c r="AK21" s="3" t="n">
+      <c r="AK21" s="4" t="n">
         <v>14.3075453677173</v>
       </c>
-      <c r="AL21" s="3" t="n">
+      <c r="AL21" s="4" t="n">
         <v>2.46211210007217</v>
       </c>
-      <c r="AM21" s="3" t="n">
+      <c r="AM21" s="4" t="n">
         <v>2.46211210007217</v>
       </c>
-      <c r="AN21" s="3" t="n">
+      <c r="AN21" s="4" t="n">
         <v>2.46211210007217</v>
       </c>
-      <c r="AO21" s="3" t="n">
+      <c r="AO21" s="4" t="n">
         <v>2.46211210007217</v>
       </c>
-      <c r="AP21" s="3" t="n">
+      <c r="AP21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AQ21" s="3" t="n">
+      <c r="AQ21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AR21" s="3" t="n">
+      <c r="AR21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AS21" s="3" t="n">
+      <c r="AS21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="AT21" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="AZ21" s="3" t="n">
+      <c r="AZ21" s="4" t="n">
         <v>0.629072118625028</v>
       </c>
-      <c r="BA21" s="3" t="n">
+      <c r="BA21" s="4" t="n">
         <v>46.2397540983607</v>
       </c>
       <c r="BB21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="BG21" s="3" t="n">
+      <c r="BG21" s="4" t="n">
         <v>18.8385598141696</v>
       </c>
-      <c r="BH21" s="3" t="n">
+      <c r="BH21" s="4" t="n">
         <v>18.8385598141696</v>
       </c>
-      <c r="BK21" s="3" t="n">
+      <c r="BK21" s="4" t="n">
         <v>12</v>
       </c>
       <c r="BM21" s="0" t="n">
@@ -3041,115 +3052,115 @@
       <c r="A22" s="1" t="n">
         <v>44495</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>0.760462465396515</v>
       </c>
-      <c r="G22" s="3" t="n">
+      <c r="G22" s="4" t="n">
         <v>3.4273344254622</v>
       </c>
-      <c r="I22" s="3" t="n">
+      <c r="I22" s="4" t="n">
         <v>1.59584513692162</v>
       </c>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="4" t="n">
         <v>0.127424250218633</v>
       </c>
-      <c r="M22" s="3" t="n">
+      <c r="M22" s="4" t="n">
         <v>0.127424250218633</v>
       </c>
-      <c r="N22" s="3" t="n">
+      <c r="N22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O22" s="3" t="n">
+      <c r="O22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P22" s="3" t="n">
+      <c r="P22" s="4" t="n">
         <v>0.433487012256831</v>
       </c>
-      <c r="Q22" s="3" t="n">
+      <c r="Q22" s="4" t="n">
         <v>0.433487012256831</v>
       </c>
-      <c r="R22" s="3" t="n">
+      <c r="R22" s="4" t="n">
         <v>2.98013245033113</v>
       </c>
-      <c r="T22" s="3" t="n">
+      <c r="T22" s="4" t="n">
         <v>0.933576452201094</v>
       </c>
-      <c r="V22" s="3" t="n">
+      <c r="V22" s="4" t="n">
         <v>8.89436313577742</v>
       </c>
-      <c r="W22" s="3" t="n">
+      <c r="W22" s="4" t="n">
         <v>3.37358784573432</v>
       </c>
-      <c r="AB22" s="3" t="n">
+      <c r="AB22" s="4" t="n">
         <v>0.511047788106694</v>
       </c>
-      <c r="AD22" s="3" t="n">
+      <c r="AD22" s="4" t="n">
         <v>0.30644593166608</v>
       </c>
       <c r="AE22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AF22" s="3" t="n">
+      <c r="AF22" s="4" t="n">
         <v>24.2835595776772</v>
       </c>
-      <c r="AH22" s="3" t="n">
+      <c r="AH22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AI22" s="3" t="n">
+      <c r="AI22" s="4" t="n">
         <v>0.428724544480172</v>
       </c>
-      <c r="AK22" s="3" t="n">
+      <c r="AK22" s="4" t="n">
         <v>3.54077253218884</v>
       </c>
-      <c r="AL22" s="3" t="n">
+      <c r="AL22" s="4" t="n">
         <v>0.94430265725867</v>
       </c>
-      <c r="AM22" s="3" t="n">
+      <c r="AM22" s="4" t="n">
         <v>0.94430265725867</v>
       </c>
-      <c r="AN22" s="3" t="n">
+      <c r="AN22" s="4" t="n">
         <v>0.94430265725867</v>
       </c>
-      <c r="AO22" s="3" t="n">
+      <c r="AO22" s="4" t="n">
         <v>0.94430265725867</v>
       </c>
-      <c r="AP22" s="3" t="n">
+      <c r="AP22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AQ22" s="3" t="n">
+      <c r="AQ22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AR22" s="3" t="n">
+      <c r="AR22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AS22" s="3" t="n">
+      <c r="AS22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="AT22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AZ22" s="3" t="n">
+      <c r="AZ22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="BA22" s="3" t="n">
+      <c r="BA22" s="4" t="n">
         <v>8.56756756756757</v>
       </c>
       <c r="BB22" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="BG22" s="3" t="n">
+      <c r="BG22" s="4" t="n">
         <v>2.65946502057613</v>
       </c>
-      <c r="BH22" s="3" t="n">
+      <c r="BH22" s="4" t="n">
         <v>2.65946502057613</v>
       </c>
-      <c r="BK22" s="3" t="n">
+      <c r="BK22" s="4" t="n">
         <v>2.64705882352941</v>
       </c>
       <c r="BM22" s="0" t="n">
@@ -3160,128 +3171,128 @@
       <c r="A23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="3"/>
-      <c r="C35" s="7"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3"/>
-      <c r="C36" s="5"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3"/>
-      <c r="C43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3"/>
-      <c r="C45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="3"/>
-      <c r="C48" s="6"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="3"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="3"/>
-      <c r="C50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="3"/>
-      <c r="C51" s="6"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="3"/>
-      <c r="C52" s="7"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="3"/>
-      <c r="C54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>